<commit_message>
Fixed the failing tests
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-pm-data-request-with-meters.xlsx
+++ b/seed/data_importer/tests/data/example-pm-data-request-with-meters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heslinge/Repos/seed/seed/data_importer/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achapin/seed/seed/data_importer/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496CBD0A-46BE-2C44-BB61-4D7C3C07F96A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F615E868-6E56-2945-9CAE-E6E799BEDF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information and Metrics" sheetId="1" r:id="rId1"/>
@@ -122,9 +122,6 @@
     <t>Month</t>
   </si>
   <si>
-    <t>Electricity Use (Grid)  (kBtu)</t>
-  </si>
-  <si>
     <t>Jan-16</t>
   </si>
   <si>
@@ -144,13 +141,16 @@
   </si>
   <si>
     <t>Apr-16</t>
+  </si>
+  <si>
+    <t>Electricity Use (Grid) (kBtu)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -171,6 +171,12 @@
       <b/>
       <sz val="9"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -208,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -224,6 +230,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -790,7 +799,7 @@
   <dimension ref="A1:F137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -829,8 +838,8 @@
       <c r="E5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>33</v>
+      <c r="F5" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1">
@@ -847,10 +856,10 @@
         <v>11</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" customHeight="1">
@@ -867,10 +876,10 @@
         <v>11</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" customHeight="1">
@@ -887,10 +896,10 @@
         <v>11</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" customHeight="1">
@@ -907,10 +916,10 @@
         <v>11</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1">

</xml_diff>

<commit_message>
use strip in MCM parser for XLSX headers
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-pm-data-request-with-meters.xlsx
+++ b/seed/data_importer/tests/data/example-pm-data-request-with-meters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achapin/seed/seed/data_importer/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlong/working/seed/seed/seed/data_importer/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F615E868-6E56-2945-9CAE-E6E799BEDF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E016EBDA-ADFB-E547-9099-242CD9D9F562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13580" yWindow="4600" windowWidth="38400" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information and Metrics" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="42">
   <si>
     <t>Report with Meters</t>
   </si>
@@ -119,9 +119,6 @@
     <t>BETTER integration test building</t>
   </si>
   <si>
-    <t>Month</t>
-  </si>
-  <si>
     <t>Jan-16</t>
   </si>
   <si>
@@ -143,14 +140,20 @@
     <t>Apr-16</t>
   </si>
   <si>
-    <t>Electricity Use (Grid) (kBtu)</t>
+    <t xml:space="preserve">Month </t>
+  </si>
+  <si>
+    <t>Electricity Use (Grid)  (kBtu)</t>
+  </si>
+  <si>
+    <t>1/13/2022 - NL: Updated with extra space after month.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -162,15 +165,12 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -214,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -230,9 +230,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,32 +552,32 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="60" customHeight="1">
+    <row r="6" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -597,7 +594,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" customHeight="1">
+    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -614,7 +611,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" customHeight="1">
+    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -631,7 +628,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" customHeight="1">
+    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
@@ -648,7 +645,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1">
+    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -665,7 +662,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" customHeight="1">
+    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -682,7 +679,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1">
+    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
@@ -699,7 +696,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" customHeight="1">
+    <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
@@ -716,7 +713,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" customHeight="1">
+    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
@@ -733,7 +730,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" customHeight="1">
+    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
@@ -750,7 +747,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" customHeight="1">
+    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>28</v>
       </c>
@@ -767,7 +764,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" customHeight="1">
+    <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>30</v>
       </c>
@@ -798,31 +795,34 @@
   </sheetPr>
   <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="60" customHeight="1">
+    <row r="5" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -836,13 +836,13 @@
         <v>7</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1">
+    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -856,13 +856,13 @@
         <v>11</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" customHeight="1">
+    </row>
+    <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -876,13 +876,13 @@
         <v>11</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" customHeight="1">
+    </row>
+    <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -896,13 +896,13 @@
         <v>11</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" customHeight="1">
+    </row>
+    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -916,13 +916,13 @@
         <v>11</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -930,7 +930,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="30" customHeight="1">
+    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -938,7 +938,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="30" customHeight="1">
+    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -946,7 +946,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="30" customHeight="1">
+    <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -954,7 +954,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="30" customHeight="1">
+    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -962,7 +962,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="30" customHeight="1">
+    <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -970,7 +970,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="30" customHeight="1">
+    <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -978,7 +978,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="30" customHeight="1">
+    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -986,7 +986,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="30" customHeight="1">
+    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -994,7 +994,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="30" customHeight="1">
+    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1002,7 +1002,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="30" customHeight="1">
+    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1010,7 +1010,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="30" customHeight="1">
+    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1018,7 +1018,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="30" customHeight="1">
+    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1026,7 +1026,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="30" customHeight="1">
+    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1034,7 +1034,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="30" customHeight="1">
+    <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1042,7 +1042,7 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" ht="30" customHeight="1">
+    <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1050,7 +1050,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="30" customHeight="1">
+    <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1058,7 +1058,7 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="30" customHeight="1">
+    <row r="27" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1066,7 +1066,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="30" customHeight="1">
+    <row r="28" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1074,7 +1074,7 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" ht="30" customHeight="1">
+    <row r="29" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1082,7 +1082,7 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="30" customHeight="1">
+    <row r="30" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1090,7 +1090,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" ht="30" customHeight="1">
+    <row r="31" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1098,7 +1098,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" ht="30" customHeight="1">
+    <row r="32" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1106,7 +1106,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" ht="30" customHeight="1">
+    <row r="33" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1114,7 +1114,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" ht="30" customHeight="1">
+    <row r="34" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1122,7 +1122,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" ht="30" customHeight="1">
+    <row r="35" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1130,7 +1130,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" ht="30" customHeight="1">
+    <row r="36" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1138,7 +1138,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" ht="30" customHeight="1">
+    <row r="37" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1146,7 +1146,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" ht="30" customHeight="1">
+    <row r="38" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1154,7 +1154,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" ht="30" customHeight="1">
+    <row r="39" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1162,7 +1162,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" ht="30" customHeight="1">
+    <row r="40" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1170,7 +1170,7 @@
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" ht="30" customHeight="1">
+    <row r="41" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1178,7 +1178,7 @@
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:6" ht="30" customHeight="1">
+    <row r="42" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1186,7 +1186,7 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:6" ht="30" customHeight="1">
+    <row r="43" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1194,7 +1194,7 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:6" ht="30" customHeight="1">
+    <row r="44" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -1202,7 +1202,7 @@
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:6" ht="30" customHeight="1">
+    <row r="45" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -1210,7 +1210,7 @@
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="1:6" ht="30" customHeight="1">
+    <row r="46" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -1218,7 +1218,7 @@
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:6" ht="30" customHeight="1">
+    <row r="47" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -1226,7 +1226,7 @@
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="1:6" ht="30" customHeight="1">
+    <row r="48" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -1234,7 +1234,7 @@
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="1:6" ht="30" customHeight="1">
+    <row r="49" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -1242,7 +1242,7 @@
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
     </row>
-    <row r="50" spans="1:6" ht="30" customHeight="1">
+    <row r="50" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -1250,7 +1250,7 @@
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
     </row>
-    <row r="51" spans="1:6" ht="30" customHeight="1">
+    <row r="51" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -1258,7 +1258,7 @@
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" spans="1:6" ht="30" customHeight="1">
+    <row r="52" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -1266,7 +1266,7 @@
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" spans="1:6" ht="30" customHeight="1">
+    <row r="53" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -1274,7 +1274,7 @@
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
     </row>
-    <row r="54" spans="1:6" ht="30" customHeight="1">
+    <row r="54" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -1282,7 +1282,7 @@
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
     </row>
-    <row r="55" spans="1:6" ht="30" customHeight="1">
+    <row r="55" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -1290,7 +1290,7 @@
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
     </row>
-    <row r="56" spans="1:6" ht="30" customHeight="1">
+    <row r="56" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -1298,7 +1298,7 @@
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
     </row>
-    <row r="57" spans="1:6" ht="30" customHeight="1">
+    <row r="57" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -1306,7 +1306,7 @@
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" spans="1:6" ht="30" customHeight="1">
+    <row r="58" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -1314,7 +1314,7 @@
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
     </row>
-    <row r="59" spans="1:6" ht="30" customHeight="1">
+    <row r="59" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -1322,7 +1322,7 @@
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
     </row>
-    <row r="60" spans="1:6" ht="30" customHeight="1">
+    <row r="60" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -1330,7 +1330,7 @@
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
     </row>
-    <row r="61" spans="1:6" ht="30" customHeight="1">
+    <row r="61" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -1338,7 +1338,7 @@
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
     </row>
-    <row r="62" spans="1:6" ht="30" customHeight="1">
+    <row r="62" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -1346,7 +1346,7 @@
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
     </row>
-    <row r="63" spans="1:6" ht="30" customHeight="1">
+    <row r="63" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -1354,7 +1354,7 @@
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
     </row>
-    <row r="64" spans="1:6" ht="30" customHeight="1">
+    <row r="64" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -1362,7 +1362,7 @@
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
     </row>
-    <row r="65" spans="1:6" ht="30" customHeight="1">
+    <row r="65" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -1370,7 +1370,7 @@
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
     </row>
-    <row r="66" spans="1:6" ht="30" customHeight="1">
+    <row r="66" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -1378,7 +1378,7 @@
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
     </row>
-    <row r="67" spans="1:6" ht="30" customHeight="1">
+    <row r="67" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -1386,7 +1386,7 @@
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
     </row>
-    <row r="68" spans="1:6" ht="30" customHeight="1">
+    <row r="68" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -1394,7 +1394,7 @@
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
     </row>
-    <row r="69" spans="1:6" ht="30" customHeight="1">
+    <row r="69" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -1402,7 +1402,7 @@
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
     </row>
-    <row r="70" spans="1:6" ht="30" customHeight="1">
+    <row r="70" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -1410,7 +1410,7 @@
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
     </row>
-    <row r="71" spans="1:6" ht="30" customHeight="1">
+    <row r="71" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -1418,7 +1418,7 @@
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
     </row>
-    <row r="72" spans="1:6" ht="30" customHeight="1">
+    <row r="72" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -1426,7 +1426,7 @@
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
     </row>
-    <row r="73" spans="1:6" ht="30" customHeight="1">
+    <row r="73" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -1434,7 +1434,7 @@
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
     </row>
-    <row r="74" spans="1:6" ht="30" customHeight="1">
+    <row r="74" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -1442,7 +1442,7 @@
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
     </row>
-    <row r="75" spans="1:6" ht="30" customHeight="1">
+    <row r="75" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -1450,7 +1450,7 @@
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
     </row>
-    <row r="76" spans="1:6" ht="30" customHeight="1">
+    <row r="76" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -1458,7 +1458,7 @@
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
     </row>
-    <row r="77" spans="1:6" ht="30" customHeight="1">
+    <row r="77" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -1466,7 +1466,7 @@
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
     </row>
-    <row r="78" spans="1:6" ht="30" customHeight="1">
+    <row r="78" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -1474,7 +1474,7 @@
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
     </row>
-    <row r="79" spans="1:6" ht="30" customHeight="1">
+    <row r="79" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -1482,7 +1482,7 @@
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
     </row>
-    <row r="80" spans="1:6" ht="30" customHeight="1">
+    <row r="80" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -1490,7 +1490,7 @@
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
     </row>
-    <row r="81" spans="1:6" ht="30" customHeight="1">
+    <row r="81" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -1498,7 +1498,7 @@
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
     </row>
-    <row r="82" spans="1:6" ht="30" customHeight="1">
+    <row r="82" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -1506,7 +1506,7 @@
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
     </row>
-    <row r="83" spans="1:6" ht="30" customHeight="1">
+    <row r="83" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -1514,7 +1514,7 @@
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
     </row>
-    <row r="84" spans="1:6" ht="30" customHeight="1">
+    <row r="84" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -1522,7 +1522,7 @@
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
     </row>
-    <row r="85" spans="1:6" ht="30" customHeight="1">
+    <row r="85" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -1530,7 +1530,7 @@
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
     </row>
-    <row r="86" spans="1:6" ht="30" customHeight="1">
+    <row r="86" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -1538,7 +1538,7 @@
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
     </row>
-    <row r="87" spans="1:6" ht="30" customHeight="1">
+    <row r="87" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -1546,7 +1546,7 @@
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
     </row>
-    <row r="88" spans="1:6" ht="30" customHeight="1">
+    <row r="88" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -1554,7 +1554,7 @@
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
     </row>
-    <row r="89" spans="1:6" ht="30" customHeight="1">
+    <row r="89" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -1562,7 +1562,7 @@
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
     </row>
-    <row r="90" spans="1:6" ht="30" customHeight="1">
+    <row r="90" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -1570,7 +1570,7 @@
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
     </row>
-    <row r="91" spans="1:6" ht="30" customHeight="1">
+    <row r="91" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
@@ -1578,7 +1578,7 @@
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
     </row>
-    <row r="92" spans="1:6" ht="30" customHeight="1">
+    <row r="92" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
@@ -1586,7 +1586,7 @@
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
     </row>
-    <row r="93" spans="1:6" ht="30" customHeight="1">
+    <row r="93" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -1594,7 +1594,7 @@
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
     </row>
-    <row r="94" spans="1:6" ht="30" customHeight="1">
+    <row r="94" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
@@ -1602,7 +1602,7 @@
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
     </row>
-    <row r="95" spans="1:6" ht="30" customHeight="1">
+    <row r="95" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
@@ -1610,7 +1610,7 @@
       <c r="E95" s="4"/>
       <c r="F95" s="4"/>
     </row>
-    <row r="96" spans="1:6" ht="30" customHeight="1">
+    <row r="96" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
@@ -1618,7 +1618,7 @@
       <c r="E96" s="4"/>
       <c r="F96" s="4"/>
     </row>
-    <row r="97" spans="1:6" ht="30" customHeight="1">
+    <row r="97" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
@@ -1626,7 +1626,7 @@
       <c r="E97" s="4"/>
       <c r="F97" s="4"/>
     </row>
-    <row r="98" spans="1:6" ht="30" customHeight="1">
+    <row r="98" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="4"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
@@ -1634,7 +1634,7 @@
       <c r="E98" s="4"/>
       <c r="F98" s="4"/>
     </row>
-    <row r="99" spans="1:6" ht="30" customHeight="1">
+    <row r="99" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -1642,7 +1642,7 @@
       <c r="E99" s="4"/>
       <c r="F99" s="4"/>
     </row>
-    <row r="100" spans="1:6" ht="30" customHeight="1">
+    <row r="100" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
@@ -1650,7 +1650,7 @@
       <c r="E100" s="4"/>
       <c r="F100" s="4"/>
     </row>
-    <row r="101" spans="1:6" ht="30" customHeight="1">
+    <row r="101" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
@@ -1658,7 +1658,7 @@
       <c r="E101" s="4"/>
       <c r="F101" s="4"/>
     </row>
-    <row r="102" spans="1:6" ht="30" customHeight="1">
+    <row r="102" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
@@ -1666,7 +1666,7 @@
       <c r="E102" s="4"/>
       <c r="F102" s="4"/>
     </row>
-    <row r="103" spans="1:6" ht="30" customHeight="1">
+    <row r="103" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
@@ -1674,7 +1674,7 @@
       <c r="E103" s="4"/>
       <c r="F103" s="4"/>
     </row>
-    <row r="104" spans="1:6" ht="30" customHeight="1">
+    <row r="104" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
@@ -1682,7 +1682,7 @@
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
     </row>
-    <row r="105" spans="1:6" ht="30" customHeight="1">
+    <row r="105" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
@@ -1690,7 +1690,7 @@
       <c r="E105" s="4"/>
       <c r="F105" s="4"/>
     </row>
-    <row r="106" spans="1:6" ht="30" customHeight="1">
+    <row r="106" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
@@ -1698,7 +1698,7 @@
       <c r="E106" s="4"/>
       <c r="F106" s="4"/>
     </row>
-    <row r="107" spans="1:6" ht="30" customHeight="1">
+    <row r="107" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
@@ -1706,7 +1706,7 @@
       <c r="E107" s="4"/>
       <c r="F107" s="4"/>
     </row>
-    <row r="108" spans="1:6" ht="30" customHeight="1">
+    <row r="108" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
@@ -1714,7 +1714,7 @@
       <c r="E108" s="4"/>
       <c r="F108" s="4"/>
     </row>
-    <row r="109" spans="1:6" ht="30" customHeight="1">
+    <row r="109" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
@@ -1722,7 +1722,7 @@
       <c r="E109" s="4"/>
       <c r="F109" s="4"/>
     </row>
-    <row r="110" spans="1:6" ht="30" customHeight="1">
+    <row r="110" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
@@ -1730,7 +1730,7 @@
       <c r="E110" s="4"/>
       <c r="F110" s="4"/>
     </row>
-    <row r="111" spans="1:6" ht="30" customHeight="1">
+    <row r="111" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
@@ -1738,7 +1738,7 @@
       <c r="E111" s="4"/>
       <c r="F111" s="4"/>
     </row>
-    <row r="112" spans="1:6" ht="30" customHeight="1">
+    <row r="112" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
@@ -1746,7 +1746,7 @@
       <c r="E112" s="4"/>
       <c r="F112" s="4"/>
     </row>
-    <row r="113" spans="1:6" ht="30" customHeight="1">
+    <row r="113" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
@@ -1754,7 +1754,7 @@
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
     </row>
-    <row r="114" spans="1:6" ht="30" customHeight="1">
+    <row r="114" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
@@ -1762,7 +1762,7 @@
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
     </row>
-    <row r="115" spans="1:6" ht="30" customHeight="1">
+    <row r="115" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
@@ -1770,7 +1770,7 @@
       <c r="E115" s="4"/>
       <c r="F115" s="4"/>
     </row>
-    <row r="116" spans="1:6" ht="30" customHeight="1">
+    <row r="116" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
@@ -1778,7 +1778,7 @@
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>
     </row>
-    <row r="117" spans="1:6" ht="30" customHeight="1">
+    <row r="117" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
@@ -1786,7 +1786,7 @@
       <c r="E117" s="4"/>
       <c r="F117" s="4"/>
     </row>
-    <row r="118" spans="1:6" ht="30" customHeight="1">
+    <row r="118" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="4"/>
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
@@ -1794,7 +1794,7 @@
       <c r="E118" s="4"/>
       <c r="F118" s="4"/>
     </row>
-    <row r="119" spans="1:6" ht="30" customHeight="1">
+    <row r="119" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="4"/>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
@@ -1802,7 +1802,7 @@
       <c r="E119" s="4"/>
       <c r="F119" s="4"/>
     </row>
-    <row r="120" spans="1:6" ht="30" customHeight="1">
+    <row r="120" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
@@ -1810,7 +1810,7 @@
       <c r="E120" s="4"/>
       <c r="F120" s="4"/>
     </row>
-    <row r="121" spans="1:6" ht="30" customHeight="1">
+    <row r="121" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="4"/>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
@@ -1818,7 +1818,7 @@
       <c r="E121" s="4"/>
       <c r="F121" s="4"/>
     </row>
-    <row r="122" spans="1:6" ht="30" customHeight="1">
+    <row r="122" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="4"/>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
@@ -1826,7 +1826,7 @@
       <c r="E122" s="4"/>
       <c r="F122" s="4"/>
     </row>
-    <row r="123" spans="1:6" ht="30" customHeight="1">
+    <row r="123" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
@@ -1834,7 +1834,7 @@
       <c r="E123" s="4"/>
       <c r="F123" s="4"/>
     </row>
-    <row r="124" spans="1:6" ht="30" customHeight="1">
+    <row r="124" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="4"/>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
@@ -1842,7 +1842,7 @@
       <c r="E124" s="4"/>
       <c r="F124" s="4"/>
     </row>
-    <row r="125" spans="1:6" ht="30" customHeight="1">
+    <row r="125" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="4"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
@@ -1850,7 +1850,7 @@
       <c r="E125" s="4"/>
       <c r="F125" s="4"/>
     </row>
-    <row r="126" spans="1:6" ht="30" customHeight="1">
+    <row r="126" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
@@ -1858,7 +1858,7 @@
       <c r="E126" s="4"/>
       <c r="F126" s="4"/>
     </row>
-    <row r="127" spans="1:6" ht="30" customHeight="1">
+    <row r="127" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="4"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
@@ -1866,7 +1866,7 @@
       <c r="E127" s="4"/>
       <c r="F127" s="4"/>
     </row>
-    <row r="128" spans="1:6" ht="30" customHeight="1">
+    <row r="128" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
@@ -1874,7 +1874,7 @@
       <c r="E128" s="4"/>
       <c r="F128" s="4"/>
     </row>
-    <row r="129" spans="1:6" ht="30" customHeight="1">
+    <row r="129" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="4"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
@@ -1882,7 +1882,7 @@
       <c r="E129" s="4"/>
       <c r="F129" s="4"/>
     </row>
-    <row r="130" spans="1:6" ht="30" customHeight="1">
+    <row r="130" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="4"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
@@ -1890,7 +1890,7 @@
       <c r="E130" s="4"/>
       <c r="F130" s="4"/>
     </row>
-    <row r="131" spans="1:6" ht="30" customHeight="1">
+    <row r="131" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="4"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
@@ -1898,7 +1898,7 @@
       <c r="E131" s="4"/>
       <c r="F131" s="4"/>
     </row>
-    <row r="132" spans="1:6" ht="30" customHeight="1">
+    <row r="132" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="4"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
@@ -1906,7 +1906,7 @@
       <c r="E132" s="4"/>
       <c r="F132" s="4"/>
     </row>
-    <row r="133" spans="1:6" ht="30" customHeight="1">
+    <row r="133" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="4"/>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
@@ -1914,7 +1914,7 @@
       <c r="E133" s="4"/>
       <c r="F133" s="4"/>
     </row>
-    <row r="134" spans="1:6" ht="30" customHeight="1">
+    <row r="134" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="4"/>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
@@ -1922,7 +1922,7 @@
       <c r="E134" s="4"/>
       <c r="F134" s="4"/>
     </row>
-    <row r="135" spans="1:6" ht="30" customHeight="1">
+    <row r="135" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="4"/>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
@@ -1930,7 +1930,7 @@
       <c r="E135" s="4"/>
       <c r="F135" s="4"/>
     </row>
-    <row r="136" spans="1:6" ht="30" customHeight="1">
+    <row r="136" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="4"/>
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
@@ -1938,7 +1938,7 @@
       <c r="E136" s="4"/>
       <c r="F136" s="4"/>
     </row>
-    <row r="137" spans="1:6" ht="30" customHeight="1">
+    <row r="137" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="4"/>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>

</xml_diff>

<commit_message>
Remove all extra spaces in headers from XLSX files (#3747)
use strip in MCM parser for XLSX headers
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-pm-data-request-with-meters.xlsx
+++ b/seed/data_importer/tests/data/example-pm-data-request-with-meters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achapin/seed/seed/data_importer/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlong/working/seed/seed/seed/data_importer/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F615E868-6E56-2945-9CAE-E6E799BEDF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E016EBDA-ADFB-E547-9099-242CD9D9F562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13580" yWindow="4600" windowWidth="38400" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information and Metrics" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="42">
   <si>
     <t>Report with Meters</t>
   </si>
@@ -119,9 +119,6 @@
     <t>BETTER integration test building</t>
   </si>
   <si>
-    <t>Month</t>
-  </si>
-  <si>
     <t>Jan-16</t>
   </si>
   <si>
@@ -143,14 +140,20 @@
     <t>Apr-16</t>
   </si>
   <si>
-    <t>Electricity Use (Grid) (kBtu)</t>
+    <t xml:space="preserve">Month </t>
+  </si>
+  <si>
+    <t>Electricity Use (Grid)  (kBtu)</t>
+  </si>
+  <si>
+    <t>1/13/2022 - NL: Updated with extra space after month.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -162,15 +165,12 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -214,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -230,9 +230,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,32 +552,32 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="60" customHeight="1">
+    <row r="6" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -597,7 +594,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" customHeight="1">
+    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -614,7 +611,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" customHeight="1">
+    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -631,7 +628,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" customHeight="1">
+    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
@@ -648,7 +645,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1">
+    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -665,7 +662,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" customHeight="1">
+    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -682,7 +679,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1">
+    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
@@ -699,7 +696,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" customHeight="1">
+    <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
@@ -716,7 +713,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" customHeight="1">
+    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
@@ -733,7 +730,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" customHeight="1">
+    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
@@ -750,7 +747,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" customHeight="1">
+    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>28</v>
       </c>
@@ -767,7 +764,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" customHeight="1">
+    <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>30</v>
       </c>
@@ -798,31 +795,34 @@
   </sheetPr>
   <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="60" customHeight="1">
+    <row r="5" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -836,13 +836,13 @@
         <v>7</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1">
+    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -856,13 +856,13 @@
         <v>11</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" customHeight="1">
+    </row>
+    <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -876,13 +876,13 @@
         <v>11</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" customHeight="1">
+    </row>
+    <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -896,13 +896,13 @@
         <v>11</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" customHeight="1">
+    </row>
+    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -916,13 +916,13 @@
         <v>11</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -930,7 +930,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="30" customHeight="1">
+    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -938,7 +938,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="30" customHeight="1">
+    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -946,7 +946,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="30" customHeight="1">
+    <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -954,7 +954,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="30" customHeight="1">
+    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -962,7 +962,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="30" customHeight="1">
+    <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -970,7 +970,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="30" customHeight="1">
+    <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -978,7 +978,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="30" customHeight="1">
+    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -986,7 +986,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="30" customHeight="1">
+    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -994,7 +994,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="30" customHeight="1">
+    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1002,7 +1002,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="30" customHeight="1">
+    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1010,7 +1010,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="30" customHeight="1">
+    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1018,7 +1018,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="30" customHeight="1">
+    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1026,7 +1026,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="30" customHeight="1">
+    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1034,7 +1034,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="30" customHeight="1">
+    <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1042,7 +1042,7 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" ht="30" customHeight="1">
+    <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1050,7 +1050,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="30" customHeight="1">
+    <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1058,7 +1058,7 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="30" customHeight="1">
+    <row r="27" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1066,7 +1066,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="30" customHeight="1">
+    <row r="28" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1074,7 +1074,7 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" ht="30" customHeight="1">
+    <row r="29" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1082,7 +1082,7 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="30" customHeight="1">
+    <row r="30" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1090,7 +1090,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" ht="30" customHeight="1">
+    <row r="31" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1098,7 +1098,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" ht="30" customHeight="1">
+    <row r="32" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1106,7 +1106,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" ht="30" customHeight="1">
+    <row r="33" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1114,7 +1114,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" ht="30" customHeight="1">
+    <row r="34" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1122,7 +1122,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" ht="30" customHeight="1">
+    <row r="35" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1130,7 +1130,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" ht="30" customHeight="1">
+    <row r="36" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1138,7 +1138,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" ht="30" customHeight="1">
+    <row r="37" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1146,7 +1146,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" ht="30" customHeight="1">
+    <row r="38" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1154,7 +1154,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" ht="30" customHeight="1">
+    <row r="39" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1162,7 +1162,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" ht="30" customHeight="1">
+    <row r="40" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1170,7 +1170,7 @@
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" ht="30" customHeight="1">
+    <row r="41" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1178,7 +1178,7 @@
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:6" ht="30" customHeight="1">
+    <row r="42" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1186,7 +1186,7 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:6" ht="30" customHeight="1">
+    <row r="43" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1194,7 +1194,7 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:6" ht="30" customHeight="1">
+    <row r="44" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -1202,7 +1202,7 @@
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:6" ht="30" customHeight="1">
+    <row r="45" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -1210,7 +1210,7 @@
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="1:6" ht="30" customHeight="1">
+    <row r="46" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -1218,7 +1218,7 @@
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:6" ht="30" customHeight="1">
+    <row r="47" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -1226,7 +1226,7 @@
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="1:6" ht="30" customHeight="1">
+    <row r="48" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -1234,7 +1234,7 @@
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="1:6" ht="30" customHeight="1">
+    <row r="49" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -1242,7 +1242,7 @@
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
     </row>
-    <row r="50" spans="1:6" ht="30" customHeight="1">
+    <row r="50" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -1250,7 +1250,7 @@
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
     </row>
-    <row r="51" spans="1:6" ht="30" customHeight="1">
+    <row r="51" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -1258,7 +1258,7 @@
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" spans="1:6" ht="30" customHeight="1">
+    <row r="52" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -1266,7 +1266,7 @@
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" spans="1:6" ht="30" customHeight="1">
+    <row r="53" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -1274,7 +1274,7 @@
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
     </row>
-    <row r="54" spans="1:6" ht="30" customHeight="1">
+    <row r="54" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -1282,7 +1282,7 @@
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
     </row>
-    <row r="55" spans="1:6" ht="30" customHeight="1">
+    <row r="55" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -1290,7 +1290,7 @@
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
     </row>
-    <row r="56" spans="1:6" ht="30" customHeight="1">
+    <row r="56" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -1298,7 +1298,7 @@
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
     </row>
-    <row r="57" spans="1:6" ht="30" customHeight="1">
+    <row r="57" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -1306,7 +1306,7 @@
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" spans="1:6" ht="30" customHeight="1">
+    <row r="58" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -1314,7 +1314,7 @@
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
     </row>
-    <row r="59" spans="1:6" ht="30" customHeight="1">
+    <row r="59" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -1322,7 +1322,7 @@
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
     </row>
-    <row r="60" spans="1:6" ht="30" customHeight="1">
+    <row r="60" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -1330,7 +1330,7 @@
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
     </row>
-    <row r="61" spans="1:6" ht="30" customHeight="1">
+    <row r="61" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -1338,7 +1338,7 @@
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
     </row>
-    <row r="62" spans="1:6" ht="30" customHeight="1">
+    <row r="62" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -1346,7 +1346,7 @@
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
     </row>
-    <row r="63" spans="1:6" ht="30" customHeight="1">
+    <row r="63" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -1354,7 +1354,7 @@
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
     </row>
-    <row r="64" spans="1:6" ht="30" customHeight="1">
+    <row r="64" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -1362,7 +1362,7 @@
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
     </row>
-    <row r="65" spans="1:6" ht="30" customHeight="1">
+    <row r="65" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -1370,7 +1370,7 @@
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
     </row>
-    <row r="66" spans="1:6" ht="30" customHeight="1">
+    <row r="66" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -1378,7 +1378,7 @@
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
     </row>
-    <row r="67" spans="1:6" ht="30" customHeight="1">
+    <row r="67" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -1386,7 +1386,7 @@
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
     </row>
-    <row r="68" spans="1:6" ht="30" customHeight="1">
+    <row r="68" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -1394,7 +1394,7 @@
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
     </row>
-    <row r="69" spans="1:6" ht="30" customHeight="1">
+    <row r="69" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -1402,7 +1402,7 @@
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
     </row>
-    <row r="70" spans="1:6" ht="30" customHeight="1">
+    <row r="70" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -1410,7 +1410,7 @@
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
     </row>
-    <row r="71" spans="1:6" ht="30" customHeight="1">
+    <row r="71" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -1418,7 +1418,7 @@
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
     </row>
-    <row r="72" spans="1:6" ht="30" customHeight="1">
+    <row r="72" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -1426,7 +1426,7 @@
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
     </row>
-    <row r="73" spans="1:6" ht="30" customHeight="1">
+    <row r="73" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -1434,7 +1434,7 @@
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
     </row>
-    <row r="74" spans="1:6" ht="30" customHeight="1">
+    <row r="74" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -1442,7 +1442,7 @@
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
     </row>
-    <row r="75" spans="1:6" ht="30" customHeight="1">
+    <row r="75" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -1450,7 +1450,7 @@
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
     </row>
-    <row r="76" spans="1:6" ht="30" customHeight="1">
+    <row r="76" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -1458,7 +1458,7 @@
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
     </row>
-    <row r="77" spans="1:6" ht="30" customHeight="1">
+    <row r="77" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -1466,7 +1466,7 @@
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
     </row>
-    <row r="78" spans="1:6" ht="30" customHeight="1">
+    <row r="78" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -1474,7 +1474,7 @@
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
     </row>
-    <row r="79" spans="1:6" ht="30" customHeight="1">
+    <row r="79" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -1482,7 +1482,7 @@
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
     </row>
-    <row r="80" spans="1:6" ht="30" customHeight="1">
+    <row r="80" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -1490,7 +1490,7 @@
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
     </row>
-    <row r="81" spans="1:6" ht="30" customHeight="1">
+    <row r="81" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -1498,7 +1498,7 @@
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
     </row>
-    <row r="82" spans="1:6" ht="30" customHeight="1">
+    <row r="82" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -1506,7 +1506,7 @@
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
     </row>
-    <row r="83" spans="1:6" ht="30" customHeight="1">
+    <row r="83" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -1514,7 +1514,7 @@
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
     </row>
-    <row r="84" spans="1:6" ht="30" customHeight="1">
+    <row r="84" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -1522,7 +1522,7 @@
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
     </row>
-    <row r="85" spans="1:6" ht="30" customHeight="1">
+    <row r="85" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -1530,7 +1530,7 @@
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
     </row>
-    <row r="86" spans="1:6" ht="30" customHeight="1">
+    <row r="86" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -1538,7 +1538,7 @@
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
     </row>
-    <row r="87" spans="1:6" ht="30" customHeight="1">
+    <row r="87" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -1546,7 +1546,7 @@
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
     </row>
-    <row r="88" spans="1:6" ht="30" customHeight="1">
+    <row r="88" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -1554,7 +1554,7 @@
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
     </row>
-    <row r="89" spans="1:6" ht="30" customHeight="1">
+    <row r="89" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -1562,7 +1562,7 @@
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
     </row>
-    <row r="90" spans="1:6" ht="30" customHeight="1">
+    <row r="90" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -1570,7 +1570,7 @@
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
     </row>
-    <row r="91" spans="1:6" ht="30" customHeight="1">
+    <row r="91" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
@@ -1578,7 +1578,7 @@
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
     </row>
-    <row r="92" spans="1:6" ht="30" customHeight="1">
+    <row r="92" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
@@ -1586,7 +1586,7 @@
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
     </row>
-    <row r="93" spans="1:6" ht="30" customHeight="1">
+    <row r="93" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -1594,7 +1594,7 @@
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
     </row>
-    <row r="94" spans="1:6" ht="30" customHeight="1">
+    <row r="94" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
@@ -1602,7 +1602,7 @@
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
     </row>
-    <row r="95" spans="1:6" ht="30" customHeight="1">
+    <row r="95" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
@@ -1610,7 +1610,7 @@
       <c r="E95" s="4"/>
       <c r="F95" s="4"/>
     </row>
-    <row r="96" spans="1:6" ht="30" customHeight="1">
+    <row r="96" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
@@ -1618,7 +1618,7 @@
       <c r="E96" s="4"/>
       <c r="F96" s="4"/>
     </row>
-    <row r="97" spans="1:6" ht="30" customHeight="1">
+    <row r="97" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
@@ -1626,7 +1626,7 @@
       <c r="E97" s="4"/>
       <c r="F97" s="4"/>
     </row>
-    <row r="98" spans="1:6" ht="30" customHeight="1">
+    <row r="98" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="4"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
@@ -1634,7 +1634,7 @@
       <c r="E98" s="4"/>
       <c r="F98" s="4"/>
     </row>
-    <row r="99" spans="1:6" ht="30" customHeight="1">
+    <row r="99" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -1642,7 +1642,7 @@
       <c r="E99" s="4"/>
       <c r="F99" s="4"/>
     </row>
-    <row r="100" spans="1:6" ht="30" customHeight="1">
+    <row r="100" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
@@ -1650,7 +1650,7 @@
       <c r="E100" s="4"/>
       <c r="F100" s="4"/>
     </row>
-    <row r="101" spans="1:6" ht="30" customHeight="1">
+    <row r="101" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
@@ -1658,7 +1658,7 @@
       <c r="E101" s="4"/>
       <c r="F101" s="4"/>
     </row>
-    <row r="102" spans="1:6" ht="30" customHeight="1">
+    <row r="102" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
@@ -1666,7 +1666,7 @@
       <c r="E102" s="4"/>
       <c r="F102" s="4"/>
     </row>
-    <row r="103" spans="1:6" ht="30" customHeight="1">
+    <row r="103" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
@@ -1674,7 +1674,7 @@
       <c r="E103" s="4"/>
       <c r="F103" s="4"/>
     </row>
-    <row r="104" spans="1:6" ht="30" customHeight="1">
+    <row r="104" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
@@ -1682,7 +1682,7 @@
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
     </row>
-    <row r="105" spans="1:6" ht="30" customHeight="1">
+    <row r="105" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
@@ -1690,7 +1690,7 @@
       <c r="E105" s="4"/>
       <c r="F105" s="4"/>
     </row>
-    <row r="106" spans="1:6" ht="30" customHeight="1">
+    <row r="106" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
@@ -1698,7 +1698,7 @@
       <c r="E106" s="4"/>
       <c r="F106" s="4"/>
     </row>
-    <row r="107" spans="1:6" ht="30" customHeight="1">
+    <row r="107" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
@@ -1706,7 +1706,7 @@
       <c r="E107" s="4"/>
       <c r="F107" s="4"/>
     </row>
-    <row r="108" spans="1:6" ht="30" customHeight="1">
+    <row r="108" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
@@ -1714,7 +1714,7 @@
       <c r="E108" s="4"/>
       <c r="F108" s="4"/>
     </row>
-    <row r="109" spans="1:6" ht="30" customHeight="1">
+    <row r="109" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
@@ -1722,7 +1722,7 @@
       <c r="E109" s="4"/>
       <c r="F109" s="4"/>
     </row>
-    <row r="110" spans="1:6" ht="30" customHeight="1">
+    <row r="110" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
@@ -1730,7 +1730,7 @@
       <c r="E110" s="4"/>
       <c r="F110" s="4"/>
     </row>
-    <row r="111" spans="1:6" ht="30" customHeight="1">
+    <row r="111" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
@@ -1738,7 +1738,7 @@
       <c r="E111" s="4"/>
       <c r="F111" s="4"/>
     </row>
-    <row r="112" spans="1:6" ht="30" customHeight="1">
+    <row r="112" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
@@ -1746,7 +1746,7 @@
       <c r="E112" s="4"/>
       <c r="F112" s="4"/>
     </row>
-    <row r="113" spans="1:6" ht="30" customHeight="1">
+    <row r="113" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
@@ -1754,7 +1754,7 @@
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
     </row>
-    <row r="114" spans="1:6" ht="30" customHeight="1">
+    <row r="114" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
@@ -1762,7 +1762,7 @@
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
     </row>
-    <row r="115" spans="1:6" ht="30" customHeight="1">
+    <row r="115" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
@@ -1770,7 +1770,7 @@
       <c r="E115" s="4"/>
       <c r="F115" s="4"/>
     </row>
-    <row r="116" spans="1:6" ht="30" customHeight="1">
+    <row r="116" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
@@ -1778,7 +1778,7 @@
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>
     </row>
-    <row r="117" spans="1:6" ht="30" customHeight="1">
+    <row r="117" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
@@ -1786,7 +1786,7 @@
       <c r="E117" s="4"/>
       <c r="F117" s="4"/>
     </row>
-    <row r="118" spans="1:6" ht="30" customHeight="1">
+    <row r="118" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="4"/>
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
@@ -1794,7 +1794,7 @@
       <c r="E118" s="4"/>
       <c r="F118" s="4"/>
     </row>
-    <row r="119" spans="1:6" ht="30" customHeight="1">
+    <row r="119" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="4"/>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
@@ -1802,7 +1802,7 @@
       <c r="E119" s="4"/>
       <c r="F119" s="4"/>
     </row>
-    <row r="120" spans="1:6" ht="30" customHeight="1">
+    <row r="120" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
@@ -1810,7 +1810,7 @@
       <c r="E120" s="4"/>
       <c r="F120" s="4"/>
     </row>
-    <row r="121" spans="1:6" ht="30" customHeight="1">
+    <row r="121" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="4"/>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
@@ -1818,7 +1818,7 @@
       <c r="E121" s="4"/>
       <c r="F121" s="4"/>
     </row>
-    <row r="122" spans="1:6" ht="30" customHeight="1">
+    <row r="122" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="4"/>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
@@ -1826,7 +1826,7 @@
       <c r="E122" s="4"/>
       <c r="F122" s="4"/>
     </row>
-    <row r="123" spans="1:6" ht="30" customHeight="1">
+    <row r="123" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
@@ -1834,7 +1834,7 @@
       <c r="E123" s="4"/>
       <c r="F123" s="4"/>
     </row>
-    <row r="124" spans="1:6" ht="30" customHeight="1">
+    <row r="124" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="4"/>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
@@ -1842,7 +1842,7 @@
       <c r="E124" s="4"/>
       <c r="F124" s="4"/>
     </row>
-    <row r="125" spans="1:6" ht="30" customHeight="1">
+    <row r="125" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="4"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
@@ -1850,7 +1850,7 @@
       <c r="E125" s="4"/>
       <c r="F125" s="4"/>
     </row>
-    <row r="126" spans="1:6" ht="30" customHeight="1">
+    <row r="126" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
@@ -1858,7 +1858,7 @@
       <c r="E126" s="4"/>
       <c r="F126" s="4"/>
     </row>
-    <row r="127" spans="1:6" ht="30" customHeight="1">
+    <row r="127" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="4"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
@@ -1866,7 +1866,7 @@
       <c r="E127" s="4"/>
       <c r="F127" s="4"/>
     </row>
-    <row r="128" spans="1:6" ht="30" customHeight="1">
+    <row r="128" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
@@ -1874,7 +1874,7 @@
       <c r="E128" s="4"/>
       <c r="F128" s="4"/>
     </row>
-    <row r="129" spans="1:6" ht="30" customHeight="1">
+    <row r="129" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="4"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
@@ -1882,7 +1882,7 @@
       <c r="E129" s="4"/>
       <c r="F129" s="4"/>
     </row>
-    <row r="130" spans="1:6" ht="30" customHeight="1">
+    <row r="130" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="4"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
@@ -1890,7 +1890,7 @@
       <c r="E130" s="4"/>
       <c r="F130" s="4"/>
     </row>
-    <row r="131" spans="1:6" ht="30" customHeight="1">
+    <row r="131" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="4"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
@@ -1898,7 +1898,7 @@
       <c r="E131" s="4"/>
       <c r="F131" s="4"/>
     </row>
-    <row r="132" spans="1:6" ht="30" customHeight="1">
+    <row r="132" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="4"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
@@ -1906,7 +1906,7 @@
       <c r="E132" s="4"/>
       <c r="F132" s="4"/>
     </row>
-    <row r="133" spans="1:6" ht="30" customHeight="1">
+    <row r="133" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="4"/>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
@@ -1914,7 +1914,7 @@
       <c r="E133" s="4"/>
       <c r="F133" s="4"/>
     </row>
-    <row r="134" spans="1:6" ht="30" customHeight="1">
+    <row r="134" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="4"/>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
@@ -1922,7 +1922,7 @@
       <c r="E134" s="4"/>
       <c r="F134" s="4"/>
     </row>
-    <row r="135" spans="1:6" ht="30" customHeight="1">
+    <row r="135" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="4"/>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
@@ -1930,7 +1930,7 @@
       <c r="E135" s="4"/>
       <c r="F135" s="4"/>
     </row>
-    <row r="136" spans="1:6" ht="30" customHeight="1">
+    <row r="136" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="4"/>
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
@@ -1938,7 +1938,7 @@
       <c r="E136" s="4"/>
       <c r="F136" s="4"/>
     </row>
-    <row r="137" spans="1:6" ht="30" customHeight="1">
+    <row r="137" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="4"/>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>

</xml_diff>

<commit_message>
Revise code to make it work more generically and added a new test for new format of ESPM data
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-pm-data-request-with-meters.xlsx
+++ b/seed/data_importer/tests/data/example-pm-data-request-with-meters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlong/working/seed/seed/seed/data_importer/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achapin/seed/seed/data_importer/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E016EBDA-ADFB-E547-9099-242CD9D9F562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C540EA5-BCD5-A34F-8B23-D47DBC5801E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13580" yWindow="4600" windowWidth="38400" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information and Metrics" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="41">
   <si>
     <t>Report with Meters</t>
   </si>
@@ -140,13 +140,10 @@
     <t>Apr-16</t>
   </si>
   <si>
-    <t xml:space="preserve">Month </t>
-  </si>
-  <si>
     <t>Electricity Use (Grid)  (kBtu)</t>
   </si>
   <si>
-    <t>1/13/2022 - NL: Updated with extra space after month.</t>
+    <t>Month</t>
   </si>
 </sst>
 </file>
@@ -796,7 +793,7 @@
   <dimension ref="A1:F137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -813,9 +810,6 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -836,10 +830,10 @@
         <v>7</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixed issue with overlapping meter readings with new ESPM format (#3745)
* Fix custom report legend sort for chrome

* Removed the console log statement

* Removed startswith method and instead stripped
units off end of field string and checked equal
to header_string

* Fixed the failing tests

* Remove all extra spaces in headers from XLSX files (#3747)

use strip in MCM parser for XLSX headers

* Revise code to make it work more generically and
added a new test for new format of ESPM data

Co-authored-by: Hannah Eslinger <heslinge@nrel.gov>
Co-authored-by: Alex Chapin <alex.chapin@nrel.gov>
Co-authored-by: Nicholas Long <1907354+nllong@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-pm-data-request-with-meters.xlsx
+++ b/seed/data_importer/tests/data/example-pm-data-request-with-meters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heslinge/Repos/seed/seed/data_importer/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achapin/seed/seed/data_importer/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496CBD0A-46BE-2C44-BB61-4D7C3C07F96A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C540EA5-BCD5-A34F-8B23-D47DBC5801E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information and Metrics" sheetId="1" r:id="rId1"/>
@@ -119,38 +119,38 @@
     <t>BETTER integration test building</t>
   </si>
   <si>
+    <t>Jan-16</t>
+  </si>
+  <si>
+    <t>85887.1</t>
+  </si>
+  <si>
+    <t>Feb-16</t>
+  </si>
+  <si>
+    <t>175697.3</t>
+  </si>
+  <si>
+    <t>Mar-16</t>
+  </si>
+  <si>
+    <t>Not Available</t>
+  </si>
+  <si>
+    <t>Apr-16</t>
+  </si>
+  <si>
+    <t>Electricity Use (Grid)  (kBtu)</t>
+  </si>
+  <si>
     <t>Month</t>
-  </si>
-  <si>
-    <t>Electricity Use (Grid)  (kBtu)</t>
-  </si>
-  <si>
-    <t>Jan-16</t>
-  </si>
-  <si>
-    <t>85887.1</t>
-  </si>
-  <si>
-    <t>Feb-16</t>
-  </si>
-  <si>
-    <t>175697.3</t>
-  </si>
-  <si>
-    <t>Mar-16</t>
-  </si>
-  <si>
-    <t>Not Available</t>
-  </si>
-  <si>
-    <t>Apr-16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -162,15 +162,18 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -546,32 +549,32 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="60" customHeight="1">
+    <row r="6" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -588,7 +591,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" customHeight="1">
+    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -605,7 +608,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" customHeight="1">
+    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -622,7 +625,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" customHeight="1">
+    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
@@ -639,7 +642,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1">
+    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -656,7 +659,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" customHeight="1">
+    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -673,7 +676,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1">
+    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
@@ -690,7 +693,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" customHeight="1">
+    <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
@@ -707,7 +710,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" customHeight="1">
+    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
@@ -724,7 +727,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" customHeight="1">
+    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
@@ -741,7 +744,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" customHeight="1">
+    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>28</v>
       </c>
@@ -758,7 +761,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" customHeight="1">
+    <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>30</v>
       </c>
@@ -789,31 +792,31 @@
   </sheetPr>
   <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="60" customHeight="1">
+    <row r="5" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -827,13 +830,13 @@
         <v>7</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -847,13 +850,13 @@
         <v>11</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" customHeight="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -867,13 +870,13 @@
         <v>11</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" customHeight="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -887,13 +890,13 @@
         <v>11</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -907,13 +910,13 @@
         <v>11</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -921,7 +924,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="30" customHeight="1">
+    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -929,7 +932,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="30" customHeight="1">
+    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -937,7 +940,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="30" customHeight="1">
+    <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -945,7 +948,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="30" customHeight="1">
+    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -953,7 +956,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="30" customHeight="1">
+    <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -961,7 +964,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="30" customHeight="1">
+    <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -969,7 +972,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="30" customHeight="1">
+    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -977,7 +980,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="30" customHeight="1">
+    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -985,7 +988,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="30" customHeight="1">
+    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -993,7 +996,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="30" customHeight="1">
+    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1001,7 +1004,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="30" customHeight="1">
+    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1009,7 +1012,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="30" customHeight="1">
+    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1017,7 +1020,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="30" customHeight="1">
+    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1025,7 +1028,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="30" customHeight="1">
+    <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1033,7 +1036,7 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" ht="30" customHeight="1">
+    <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1041,7 +1044,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="30" customHeight="1">
+    <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1049,7 +1052,7 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="30" customHeight="1">
+    <row r="27" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1057,7 +1060,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="30" customHeight="1">
+    <row r="28" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1065,7 +1068,7 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" ht="30" customHeight="1">
+    <row r="29" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1073,7 +1076,7 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="30" customHeight="1">
+    <row r="30" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1081,7 +1084,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" ht="30" customHeight="1">
+    <row r="31" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1089,7 +1092,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" ht="30" customHeight="1">
+    <row r="32" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1097,7 +1100,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" ht="30" customHeight="1">
+    <row r="33" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1105,7 +1108,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" ht="30" customHeight="1">
+    <row r="34" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1113,7 +1116,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" ht="30" customHeight="1">
+    <row r="35" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1121,7 +1124,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" ht="30" customHeight="1">
+    <row r="36" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1129,7 +1132,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" ht="30" customHeight="1">
+    <row r="37" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1137,7 +1140,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" ht="30" customHeight="1">
+    <row r="38" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1145,7 +1148,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" ht="30" customHeight="1">
+    <row r="39" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1153,7 +1156,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" ht="30" customHeight="1">
+    <row r="40" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1161,7 +1164,7 @@
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" ht="30" customHeight="1">
+    <row r="41" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1169,7 +1172,7 @@
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:6" ht="30" customHeight="1">
+    <row r="42" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1177,7 +1180,7 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:6" ht="30" customHeight="1">
+    <row r="43" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1185,7 +1188,7 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:6" ht="30" customHeight="1">
+    <row r="44" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -1193,7 +1196,7 @@
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:6" ht="30" customHeight="1">
+    <row r="45" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -1201,7 +1204,7 @@
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="1:6" ht="30" customHeight="1">
+    <row r="46" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -1209,7 +1212,7 @@
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:6" ht="30" customHeight="1">
+    <row r="47" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -1217,7 +1220,7 @@
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="1:6" ht="30" customHeight="1">
+    <row r="48" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -1225,7 +1228,7 @@
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="1:6" ht="30" customHeight="1">
+    <row r="49" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -1233,7 +1236,7 @@
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
     </row>
-    <row r="50" spans="1:6" ht="30" customHeight="1">
+    <row r="50" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -1241,7 +1244,7 @@
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
     </row>
-    <row r="51" spans="1:6" ht="30" customHeight="1">
+    <row r="51" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -1249,7 +1252,7 @@
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" spans="1:6" ht="30" customHeight="1">
+    <row r="52" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -1257,7 +1260,7 @@
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" spans="1:6" ht="30" customHeight="1">
+    <row r="53" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -1265,7 +1268,7 @@
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
     </row>
-    <row r="54" spans="1:6" ht="30" customHeight="1">
+    <row r="54" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -1273,7 +1276,7 @@
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
     </row>
-    <row r="55" spans="1:6" ht="30" customHeight="1">
+    <row r="55" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -1281,7 +1284,7 @@
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
     </row>
-    <row r="56" spans="1:6" ht="30" customHeight="1">
+    <row r="56" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -1289,7 +1292,7 @@
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
     </row>
-    <row r="57" spans="1:6" ht="30" customHeight="1">
+    <row r="57" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -1297,7 +1300,7 @@
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" spans="1:6" ht="30" customHeight="1">
+    <row r="58" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -1305,7 +1308,7 @@
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
     </row>
-    <row r="59" spans="1:6" ht="30" customHeight="1">
+    <row r="59" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -1313,7 +1316,7 @@
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
     </row>
-    <row r="60" spans="1:6" ht="30" customHeight="1">
+    <row r="60" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -1321,7 +1324,7 @@
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
     </row>
-    <row r="61" spans="1:6" ht="30" customHeight="1">
+    <row r="61" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -1329,7 +1332,7 @@
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
     </row>
-    <row r="62" spans="1:6" ht="30" customHeight="1">
+    <row r="62" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -1337,7 +1340,7 @@
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
     </row>
-    <row r="63" spans="1:6" ht="30" customHeight="1">
+    <row r="63" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -1345,7 +1348,7 @@
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
     </row>
-    <row r="64" spans="1:6" ht="30" customHeight="1">
+    <row r="64" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -1353,7 +1356,7 @@
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
     </row>
-    <row r="65" spans="1:6" ht="30" customHeight="1">
+    <row r="65" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -1361,7 +1364,7 @@
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
     </row>
-    <row r="66" spans="1:6" ht="30" customHeight="1">
+    <row r="66" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -1369,7 +1372,7 @@
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
     </row>
-    <row r="67" spans="1:6" ht="30" customHeight="1">
+    <row r="67" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -1377,7 +1380,7 @@
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
     </row>
-    <row r="68" spans="1:6" ht="30" customHeight="1">
+    <row r="68" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -1385,7 +1388,7 @@
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
     </row>
-    <row r="69" spans="1:6" ht="30" customHeight="1">
+    <row r="69" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -1393,7 +1396,7 @@
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
     </row>
-    <row r="70" spans="1:6" ht="30" customHeight="1">
+    <row r="70" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -1401,7 +1404,7 @@
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
     </row>
-    <row r="71" spans="1:6" ht="30" customHeight="1">
+    <row r="71" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -1409,7 +1412,7 @@
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
     </row>
-    <row r="72" spans="1:6" ht="30" customHeight="1">
+    <row r="72" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -1417,7 +1420,7 @@
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
     </row>
-    <row r="73" spans="1:6" ht="30" customHeight="1">
+    <row r="73" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -1425,7 +1428,7 @@
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
     </row>
-    <row r="74" spans="1:6" ht="30" customHeight="1">
+    <row r="74" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -1433,7 +1436,7 @@
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
     </row>
-    <row r="75" spans="1:6" ht="30" customHeight="1">
+    <row r="75" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -1441,7 +1444,7 @@
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
     </row>
-    <row r="76" spans="1:6" ht="30" customHeight="1">
+    <row r="76" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -1449,7 +1452,7 @@
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
     </row>
-    <row r="77" spans="1:6" ht="30" customHeight="1">
+    <row r="77" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -1457,7 +1460,7 @@
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
     </row>
-    <row r="78" spans="1:6" ht="30" customHeight="1">
+    <row r="78" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -1465,7 +1468,7 @@
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
     </row>
-    <row r="79" spans="1:6" ht="30" customHeight="1">
+    <row r="79" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -1473,7 +1476,7 @@
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
     </row>
-    <row r="80" spans="1:6" ht="30" customHeight="1">
+    <row r="80" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -1481,7 +1484,7 @@
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
     </row>
-    <row r="81" spans="1:6" ht="30" customHeight="1">
+    <row r="81" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -1489,7 +1492,7 @@
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
     </row>
-    <row r="82" spans="1:6" ht="30" customHeight="1">
+    <row r="82" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -1497,7 +1500,7 @@
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
     </row>
-    <row r="83" spans="1:6" ht="30" customHeight="1">
+    <row r="83" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -1505,7 +1508,7 @@
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
     </row>
-    <row r="84" spans="1:6" ht="30" customHeight="1">
+    <row r="84" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -1513,7 +1516,7 @@
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
     </row>
-    <row r="85" spans="1:6" ht="30" customHeight="1">
+    <row r="85" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -1521,7 +1524,7 @@
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
     </row>
-    <row r="86" spans="1:6" ht="30" customHeight="1">
+    <row r="86" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -1529,7 +1532,7 @@
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
     </row>
-    <row r="87" spans="1:6" ht="30" customHeight="1">
+    <row r="87" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -1537,7 +1540,7 @@
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
     </row>
-    <row r="88" spans="1:6" ht="30" customHeight="1">
+    <row r="88" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -1545,7 +1548,7 @@
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
     </row>
-    <row r="89" spans="1:6" ht="30" customHeight="1">
+    <row r="89" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -1553,7 +1556,7 @@
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
     </row>
-    <row r="90" spans="1:6" ht="30" customHeight="1">
+    <row r="90" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -1561,7 +1564,7 @@
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
     </row>
-    <row r="91" spans="1:6" ht="30" customHeight="1">
+    <row r="91" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
@@ -1569,7 +1572,7 @@
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
     </row>
-    <row r="92" spans="1:6" ht="30" customHeight="1">
+    <row r="92" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
@@ -1577,7 +1580,7 @@
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
     </row>
-    <row r="93" spans="1:6" ht="30" customHeight="1">
+    <row r="93" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -1585,7 +1588,7 @@
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
     </row>
-    <row r="94" spans="1:6" ht="30" customHeight="1">
+    <row r="94" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
@@ -1593,7 +1596,7 @@
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
     </row>
-    <row r="95" spans="1:6" ht="30" customHeight="1">
+    <row r="95" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
@@ -1601,7 +1604,7 @@
       <c r="E95" s="4"/>
       <c r="F95" s="4"/>
     </row>
-    <row r="96" spans="1:6" ht="30" customHeight="1">
+    <row r="96" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
@@ -1609,7 +1612,7 @@
       <c r="E96" s="4"/>
       <c r="F96" s="4"/>
     </row>
-    <row r="97" spans="1:6" ht="30" customHeight="1">
+    <row r="97" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
@@ -1617,7 +1620,7 @@
       <c r="E97" s="4"/>
       <c r="F97" s="4"/>
     </row>
-    <row r="98" spans="1:6" ht="30" customHeight="1">
+    <row r="98" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="4"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
@@ -1625,7 +1628,7 @@
       <c r="E98" s="4"/>
       <c r="F98" s="4"/>
     </row>
-    <row r="99" spans="1:6" ht="30" customHeight="1">
+    <row r="99" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -1633,7 +1636,7 @@
       <c r="E99" s="4"/>
       <c r="F99" s="4"/>
     </row>
-    <row r="100" spans="1:6" ht="30" customHeight="1">
+    <row r="100" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
@@ -1641,7 +1644,7 @@
       <c r="E100" s="4"/>
       <c r="F100" s="4"/>
     </row>
-    <row r="101" spans="1:6" ht="30" customHeight="1">
+    <row r="101" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
@@ -1649,7 +1652,7 @@
       <c r="E101" s="4"/>
       <c r="F101" s="4"/>
     </row>
-    <row r="102" spans="1:6" ht="30" customHeight="1">
+    <row r="102" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
@@ -1657,7 +1660,7 @@
       <c r="E102" s="4"/>
       <c r="F102" s="4"/>
     </row>
-    <row r="103" spans="1:6" ht="30" customHeight="1">
+    <row r="103" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
@@ -1665,7 +1668,7 @@
       <c r="E103" s="4"/>
       <c r="F103" s="4"/>
     </row>
-    <row r="104" spans="1:6" ht="30" customHeight="1">
+    <row r="104" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
@@ -1673,7 +1676,7 @@
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
     </row>
-    <row r="105" spans="1:6" ht="30" customHeight="1">
+    <row r="105" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
@@ -1681,7 +1684,7 @@
       <c r="E105" s="4"/>
       <c r="F105" s="4"/>
     </row>
-    <row r="106" spans="1:6" ht="30" customHeight="1">
+    <row r="106" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
@@ -1689,7 +1692,7 @@
       <c r="E106" s="4"/>
       <c r="F106" s="4"/>
     </row>
-    <row r="107" spans="1:6" ht="30" customHeight="1">
+    <row r="107" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
@@ -1697,7 +1700,7 @@
       <c r="E107" s="4"/>
       <c r="F107" s="4"/>
     </row>
-    <row r="108" spans="1:6" ht="30" customHeight="1">
+    <row r="108" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
@@ -1705,7 +1708,7 @@
       <c r="E108" s="4"/>
       <c r="F108" s="4"/>
     </row>
-    <row r="109" spans="1:6" ht="30" customHeight="1">
+    <row r="109" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
@@ -1713,7 +1716,7 @@
       <c r="E109" s="4"/>
       <c r="F109" s="4"/>
     </row>
-    <row r="110" spans="1:6" ht="30" customHeight="1">
+    <row r="110" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
@@ -1721,7 +1724,7 @@
       <c r="E110" s="4"/>
       <c r="F110" s="4"/>
     </row>
-    <row r="111" spans="1:6" ht="30" customHeight="1">
+    <row r="111" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
@@ -1729,7 +1732,7 @@
       <c r="E111" s="4"/>
       <c r="F111" s="4"/>
     </row>
-    <row r="112" spans="1:6" ht="30" customHeight="1">
+    <row r="112" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
@@ -1737,7 +1740,7 @@
       <c r="E112" s="4"/>
       <c r="F112" s="4"/>
     </row>
-    <row r="113" spans="1:6" ht="30" customHeight="1">
+    <row r="113" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
@@ -1745,7 +1748,7 @@
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
     </row>
-    <row r="114" spans="1:6" ht="30" customHeight="1">
+    <row r="114" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
@@ -1753,7 +1756,7 @@
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
     </row>
-    <row r="115" spans="1:6" ht="30" customHeight="1">
+    <row r="115" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
@@ -1761,7 +1764,7 @@
       <c r="E115" s="4"/>
       <c r="F115" s="4"/>
     </row>
-    <row r="116" spans="1:6" ht="30" customHeight="1">
+    <row r="116" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
@@ -1769,7 +1772,7 @@
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>
     </row>
-    <row r="117" spans="1:6" ht="30" customHeight="1">
+    <row r="117" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
@@ -1777,7 +1780,7 @@
       <c r="E117" s="4"/>
       <c r="F117" s="4"/>
     </row>
-    <row r="118" spans="1:6" ht="30" customHeight="1">
+    <row r="118" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="4"/>
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
@@ -1785,7 +1788,7 @@
       <c r="E118" s="4"/>
       <c r="F118" s="4"/>
     </row>
-    <row r="119" spans="1:6" ht="30" customHeight="1">
+    <row r="119" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="4"/>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
@@ -1793,7 +1796,7 @@
       <c r="E119" s="4"/>
       <c r="F119" s="4"/>
     </row>
-    <row r="120" spans="1:6" ht="30" customHeight="1">
+    <row r="120" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
@@ -1801,7 +1804,7 @@
       <c r="E120" s="4"/>
       <c r="F120" s="4"/>
     </row>
-    <row r="121" spans="1:6" ht="30" customHeight="1">
+    <row r="121" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="4"/>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
@@ -1809,7 +1812,7 @@
       <c r="E121" s="4"/>
       <c r="F121" s="4"/>
     </row>
-    <row r="122" spans="1:6" ht="30" customHeight="1">
+    <row r="122" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="4"/>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
@@ -1817,7 +1820,7 @@
       <c r="E122" s="4"/>
       <c r="F122" s="4"/>
     </row>
-    <row r="123" spans="1:6" ht="30" customHeight="1">
+    <row r="123" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
@@ -1825,7 +1828,7 @@
       <c r="E123" s="4"/>
       <c r="F123" s="4"/>
     </row>
-    <row r="124" spans="1:6" ht="30" customHeight="1">
+    <row r="124" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="4"/>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
@@ -1833,7 +1836,7 @@
       <c r="E124" s="4"/>
       <c r="F124" s="4"/>
     </row>
-    <row r="125" spans="1:6" ht="30" customHeight="1">
+    <row r="125" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="4"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
@@ -1841,7 +1844,7 @@
       <c r="E125" s="4"/>
       <c r="F125" s="4"/>
     </row>
-    <row r="126" spans="1:6" ht="30" customHeight="1">
+    <row r="126" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
@@ -1849,7 +1852,7 @@
       <c r="E126" s="4"/>
       <c r="F126" s="4"/>
     </row>
-    <row r="127" spans="1:6" ht="30" customHeight="1">
+    <row r="127" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="4"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
@@ -1857,7 +1860,7 @@
       <c r="E127" s="4"/>
       <c r="F127" s="4"/>
     </row>
-    <row r="128" spans="1:6" ht="30" customHeight="1">
+    <row r="128" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
@@ -1865,7 +1868,7 @@
       <c r="E128" s="4"/>
       <c r="F128" s="4"/>
     </row>
-    <row r="129" spans="1:6" ht="30" customHeight="1">
+    <row r="129" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="4"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
@@ -1873,7 +1876,7 @@
       <c r="E129" s="4"/>
       <c r="F129" s="4"/>
     </row>
-    <row r="130" spans="1:6" ht="30" customHeight="1">
+    <row r="130" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="4"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
@@ -1881,7 +1884,7 @@
       <c r="E130" s="4"/>
       <c r="F130" s="4"/>
     </row>
-    <row r="131" spans="1:6" ht="30" customHeight="1">
+    <row r="131" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="4"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
@@ -1889,7 +1892,7 @@
       <c r="E131" s="4"/>
       <c r="F131" s="4"/>
     </row>
-    <row r="132" spans="1:6" ht="30" customHeight="1">
+    <row r="132" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="4"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
@@ -1897,7 +1900,7 @@
       <c r="E132" s="4"/>
       <c r="F132" s="4"/>
     </row>
-    <row r="133" spans="1:6" ht="30" customHeight="1">
+    <row r="133" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="4"/>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
@@ -1905,7 +1908,7 @@
       <c r="E133" s="4"/>
       <c r="F133" s="4"/>
     </row>
-    <row r="134" spans="1:6" ht="30" customHeight="1">
+    <row r="134" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="4"/>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
@@ -1913,7 +1916,7 @@
       <c r="E134" s="4"/>
       <c r="F134" s="4"/>
     </row>
-    <row r="135" spans="1:6" ht="30" customHeight="1">
+    <row r="135" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="4"/>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
@@ -1921,7 +1924,7 @@
       <c r="E135" s="4"/>
       <c r="F135" s="4"/>
     </row>
-    <row r="136" spans="1:6" ht="30" customHeight="1">
+    <row r="136" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="4"/>
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
@@ -1929,7 +1932,7 @@
       <c r="E136" s="4"/>
       <c r="F136" s="4"/>
     </row>
-    <row r="137" spans="1:6" ht="30" customHeight="1">
+    <row r="137" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="4"/>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>

</xml_diff>